<commit_message>
api cridada, turnId i drawing
</commit_message>
<xml_diff>
--- a/firestorevars.xlsx
+++ b/firestorevars.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>closedRoom:Boolean</t>
   </si>
@@ -47,9 +47,6 @@
     <t>avatar:String</t>
   </si>
   <si>
-    <t>tournId:Number</t>
-  </si>
-  <si>
     <t>nombre sala creada(:string)</t>
   </si>
   <si>
@@ -66,6 +63,15 @@
   </si>
   <si>
     <t>VARIABLES CREADAS EN LA PARTE DE INICIO (HASTA PARTE AMARILLA)</t>
+  </si>
+  <si>
+    <t>drawing:null (demanar per celeste)</t>
+  </si>
+  <si>
+    <t>phrase:string(conté la frase)</t>
+  </si>
+  <si>
+    <t>turnId:Number(demanat per Oriol)</t>
   </si>
 </sst>
 </file>
@@ -156,11 +162,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,63 +459,63 @@
     <col min="2" max="2" width="34.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="5" max="5" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="5" t="s">
-        <v>11</v>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -527,12 +533,12 @@
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E12" t="s">
@@ -554,7 +560,19 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>